<commit_message>
Upload block diagram for master and slave
</commit_message>
<xml_diff>
--- a/HW/1_Design documents/MCU_Pinout.xlsx
+++ b/HW/1_Design documents/MCU_Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9068b3d81be815ab/download/New/download/Documentos/GitHub/CAPACIMETER/HW/1_Design documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_F25DC773A252ABDACC104890C15B46FA5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AFF440B-0FC8-461F-9B59-425666A44649}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC104890C15B46FA5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D263DD85-38FD-41D6-8B26-A6FFB2A1AB07}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -292,10 +292,10 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>229306</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>57800</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>208557</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -319,7 +319,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3143250" y="352425"/>
-          <a:ext cx="5058481" cy="4658375"/>
+          <a:ext cx="5647332" cy="5200650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
correct typo master block diagram
</commit_message>
<xml_diff>
--- a/HW/1_Design documents/MCU_Pinout.xlsx
+++ b/HW/1_Design documents/MCU_Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9068b3d81be815ab/download/New/download/Documentos/GitHub/CAPACIMETER/HW/1_Design documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC104890C15B46FA5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D263DD85-38FD-41D6-8B26-A6FFB2A1AB07}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="11_F25DC773A252ABDACC104890C15B46FA5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{155C65C7-63D2-44BB-9246-025633A9CC26}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
   <si>
     <t>MCU Pin Name</t>
   </si>
@@ -90,9 +90,6 @@
     <t>PC5</t>
   </si>
   <si>
-    <t>PB0</t>
-  </si>
-  <si>
     <t>PB1</t>
   </si>
   <si>
@@ -108,30 +105,6 @@
     <t>PE9</t>
   </si>
   <si>
-    <t>SPI1_CS_CELL1</t>
-  </si>
-  <si>
-    <t>SPI1_CS_CELL2</t>
-  </si>
-  <si>
-    <t>SPI1_CS_CELL3</t>
-  </si>
-  <si>
-    <t>SPI1_CS_CELL4</t>
-  </si>
-  <si>
-    <t>SPI1_CS_CELL5</t>
-  </si>
-  <si>
-    <t>SPI1_CS_CELL6</t>
-  </si>
-  <si>
-    <t>SPI1_CS_CELL7</t>
-  </si>
-  <si>
-    <t>SPI1_CS_CELL8</t>
-  </si>
-  <si>
     <t>PH0</t>
   </si>
   <si>
@@ -153,9 +126,6 @@
     <t>PA3</t>
   </si>
   <si>
-    <t>NTC_PCB</t>
-  </si>
-  <si>
     <t>I2C2_SDA</t>
   </si>
   <si>
@@ -165,42 +135,6 @@
     <t>PE14</t>
   </si>
   <si>
-    <t>RPM_FAN1</t>
-  </si>
-  <si>
-    <t>RPM_FAN2</t>
-  </si>
-  <si>
-    <t>PWM_FAN_1</t>
-  </si>
-  <si>
-    <t>PWM_FAN_2</t>
-  </si>
-  <si>
-    <t>PE2</t>
-  </si>
-  <si>
-    <t>PE3</t>
-  </si>
-  <si>
-    <t>PE4</t>
-  </si>
-  <si>
-    <t>PE5</t>
-  </si>
-  <si>
-    <t>USER_LED1</t>
-  </si>
-  <si>
-    <t>USER_LED2</t>
-  </si>
-  <si>
-    <t>USER_LED3</t>
-  </si>
-  <si>
-    <t>USER_LED4</t>
-  </si>
-  <si>
     <t>PA8</t>
   </si>
   <si>
@@ -211,6 +145,174 @@
   </si>
   <si>
     <t>I2C3_SDA</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Programming and debuging pin</t>
+  </si>
+  <si>
+    <t>Communications and interface</t>
+  </si>
+  <si>
+    <t>MP2770 control</t>
+  </si>
+  <si>
+    <t>ADC and DAC communication</t>
+  </si>
+  <si>
+    <t>MCP23008 GPIO expander control</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>PA2</t>
+  </si>
+  <si>
+    <t>NTC analog read for PCB temperature measure</t>
+  </si>
+  <si>
+    <t>ADC1_IN1</t>
+  </si>
+  <si>
+    <t>ADC1_IN2</t>
+  </si>
+  <si>
+    <t>ADC1_IN3</t>
+  </si>
+  <si>
+    <t>eFuse (MPQ5069) current measure</t>
+  </si>
+  <si>
+    <t>PA0</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>eFuse (MPQ5069) fault detection</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI0</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI3</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>GPIO_Output</t>
+  </si>
+  <si>
+    <t>eFuse (MPQ5069) auto pin control</t>
+  </si>
+  <si>
+    <t>External oscillator pins</t>
+  </si>
+  <si>
+    <t>PE11</t>
+  </si>
+  <si>
+    <t>PWM generator for fan control</t>
+  </si>
+  <si>
+    <t>TIM1_CH1</t>
+  </si>
+  <si>
+    <t>TIM1_CH2</t>
+  </si>
+  <si>
+    <t>TIM1_CH3</t>
+  </si>
+  <si>
+    <t>TIM1_CH4</t>
+  </si>
+  <si>
+    <t>Input compare for fan RPM feedback</t>
+  </si>
+  <si>
+    <t>PD1</t>
+  </si>
+  <si>
+    <t>PD0</t>
+  </si>
+  <si>
+    <t>PC12</t>
+  </si>
+  <si>
+    <t>PC11</t>
+  </si>
+  <si>
+    <t>User LED</t>
+  </si>
+  <si>
+    <t>PE10</t>
+  </si>
+  <si>
+    <t>PE12</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI4</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI5</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI1</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI2</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI7</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI8</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI10</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI12</t>
+  </si>
+  <si>
+    <t>MCP23008 Interrupt detection</t>
+  </si>
+  <si>
+    <t>PE15</t>
+  </si>
+  <si>
+    <t>PB12</t>
+  </si>
+  <si>
+    <t>PB13</t>
+  </si>
+  <si>
+    <t>PD8</t>
+  </si>
+  <si>
+    <t>PD9</t>
+  </si>
+  <si>
+    <t>PD10</t>
+  </si>
+  <si>
+    <t>MPC23008 /RESET control</t>
+  </si>
+  <si>
+    <t>PC14</t>
+  </si>
+  <si>
+    <t>PC15</t>
+  </si>
+  <si>
+    <t>MPQ4371 enable pin control</t>
   </si>
 </sst>
 </file>
@@ -260,10 +362,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -287,22 +392,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>208557</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>277319</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>86656</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE221151-C771-9D03-BE67-5655208024DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1851ABEC-5E28-6597-0EF4-6796C213B581}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -318,8 +423,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3143250" y="352425"/>
-          <a:ext cx="5647332" cy="5200650"/>
+          <a:off x="5724525" y="85725"/>
+          <a:ext cx="7840169" cy="6668431"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -598,264 +703,672 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C32"/>
+  <dimension ref="A2:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I4" sqref="I3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
       <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="C43" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>44</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" t="s">
-        <v>61</v>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change main sch sheet to A3
</commit_message>
<xml_diff>
--- a/HW/1_Design documents/MCU_Pinout.xlsx
+++ b/HW/1_Design documents/MCU_Pinout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9068b3d81be815ab/download/New/download/Documentos/GitHub/CAPACIMETER/HW/1_Design documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="11_F25DC773A252ABDACC104890C15B46FA5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{155C65C7-63D2-44BB-9246-025633A9CC26}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="11_F25DC773A252ABDACC104890C15B46FA5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10300F52-9281-4299-9EEC-902BCA2F755B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
   <si>
     <t>MCU Pin Name</t>
   </si>
@@ -57,15 +57,6 @@
     <t>CAN1_RX</t>
   </si>
   <si>
-    <t>PB10</t>
-  </si>
-  <si>
-    <t>I2C2_SCL</t>
-  </si>
-  <si>
-    <t>PB11</t>
-  </si>
-  <si>
     <t>PA6</t>
   </si>
   <si>
@@ -117,36 +108,15 @@
     <t>RCC_OSC_OUT</t>
   </si>
   <si>
-    <t>PB15</t>
-  </si>
-  <si>
-    <t>PB14</t>
-  </si>
-  <si>
     <t>PA3</t>
   </si>
   <si>
-    <t>I2C2_SDA</t>
-  </si>
-  <si>
     <t>PE13</t>
   </si>
   <si>
     <t>PE14</t>
   </si>
   <si>
-    <t>PA8</t>
-  </si>
-  <si>
-    <t>PC9</t>
-  </si>
-  <si>
-    <t>I2C3_SCL</t>
-  </si>
-  <si>
-    <t>I2C3_SDA</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -156,15 +126,6 @@
     <t>Communications and interface</t>
   </si>
   <si>
-    <t>MP2770 control</t>
-  </si>
-  <si>
-    <t>ADC and DAC communication</t>
-  </si>
-  <si>
-    <t>MCP23008 GPIO expander control</t>
-  </si>
-  <si>
     <t>PA1</t>
   </si>
   <si>
@@ -282,30 +243,6 @@
     <t>GPIO_EXTI12</t>
   </si>
   <si>
-    <t>MCP23008 Interrupt detection</t>
-  </si>
-  <si>
-    <t>PE15</t>
-  </si>
-  <si>
-    <t>PB12</t>
-  </si>
-  <si>
-    <t>PB13</t>
-  </si>
-  <si>
-    <t>PD8</t>
-  </si>
-  <si>
-    <t>PD9</t>
-  </si>
-  <si>
-    <t>PD10</t>
-  </si>
-  <si>
-    <t>MPC23008 /RESET control</t>
-  </si>
-  <si>
     <t>PC14</t>
   </si>
   <si>
@@ -313,6 +250,33 @@
   </si>
   <si>
     <t>MPQ4371 enable pin control</t>
+  </si>
+  <si>
+    <t>Slaves communication</t>
+  </si>
+  <si>
+    <t>/CS Slave 1</t>
+  </si>
+  <si>
+    <t>/CS Slave 2</t>
+  </si>
+  <si>
+    <t>/CS Slave 3</t>
+  </si>
+  <si>
+    <t>/CS Slave 4</t>
+  </si>
+  <si>
+    <t>/CS Slave 5</t>
+  </si>
+  <si>
+    <t>/CS Slave 6</t>
+  </si>
+  <si>
+    <t>/CS Slave 7</t>
+  </si>
+  <si>
+    <t>/CS Slave 8</t>
   </si>
 </sst>
 </file>
@@ -362,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -370,6 +334,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,55 +350,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>277319</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>86656</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1851ABEC-5E28-6597-0EF4-6796C213B581}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5724525" y="85725"/>
-          <a:ext cx="7840169" cy="6668431"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -703,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D48"/>
+  <dimension ref="A2:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I3:I4"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -738,7 +654,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -752,7 +668,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -766,7 +682,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -780,7 +696,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -788,13 +704,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -802,13 +718,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -816,13 +732,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -830,13 +746,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -844,13 +760,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -858,13 +774,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -872,13 +788,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -886,13 +802,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
         <v>49</v>
-      </c>
-      <c r="D14" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -900,13 +816,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -914,13 +830,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
         <v>51</v>
-      </c>
-      <c r="D16" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -928,13 +844,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
-        <v>56</v>
-      </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -942,13 +858,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
         <v>54</v>
       </c>
-      <c r="C18" t="s">
-        <v>57</v>
-      </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -956,13 +872,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -970,10 +886,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
         <v>61</v>
@@ -984,13 +900,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -998,13 +914,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1012,125 +928,125 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>64</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" t="s">
-        <v>69</v>
+      <c r="B25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" t="s">
-        <v>69</v>
+      <c r="B26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" t="s">
-        <v>74</v>
+      <c r="B27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" t="s">
-        <v>74</v>
+      <c r="B28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" t="s">
-        <v>74</v>
+      <c r="B29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" t="s">
-        <v>74</v>
+      <c r="B30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" t="s">
-        <v>85</v>
+      <c r="B31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1138,13 +1054,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="D32" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1152,229 +1068,60 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="D33" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" t="s">
-        <v>85</v>
+      <c r="B34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" t="s">
-        <v>85</v>
+      <c r="B35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="B36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="C37" t="s">
-        <v>83</v>
-      </c>
-      <c r="D37" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" t="s">
-        <v>60</v>
-      </c>
-      <c r="D41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" t="s">
-        <v>60</v>
-      </c>
-      <c r="D42" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>41</v>
-      </c>
-      <c r="B43" t="s">
-        <v>30</v>
-      </c>
-      <c r="C43" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>45</v>
-      </c>
-      <c r="B47" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>